<commit_message>
Added the requirement info for Friday's turn-in
</commit_message>
<xml_diff>
--- a/project/CSCE 356 Risk management assignment.xlsx
+++ b/project/CSCE 356 Risk management assignment.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="860" windowWidth="19200" windowHeight="11740" tabRatio="500"/>
@@ -70,10 +70,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -435,7 +441,7 @@
   <dimension ref="A3:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -530,7 +536,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>